<commit_message>
mock up connector in f360
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E01C9D-57BE-47FD-879E-FF846F4ADB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB126E-FB8C-4ABC-A135-57CCB6D7C44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="6015" windowWidth="28800" windowHeight="15345" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update parts list with alternatives
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB126E-FB8C-4ABC-A135-57CCB6D7C44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C9F1A2-C6D2-4A86-A87A-DEB675C273A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Price</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>USB4056-03-A</t>
+  </si>
+  <si>
+    <t>Alternative Parts</t>
+  </si>
+  <si>
+    <t>DX07S024XJ1R1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">670-2848-2-ND </t>
+  </si>
+  <si>
+    <t>SS-52400-003</t>
+  </si>
+  <si>
+    <t>380-SS-52400-003TR-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732-9618-2-ND </t>
   </si>
 </sst>
 </file>
@@ -118,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -129,6 +147,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -444,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0D2EA4-1276-4D7D-AD5E-6C96E3844A7C}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +538,52 @@
         <v>8.19</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10">
+        <v>632723300011</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update printable files and parts list
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67CD515-1A2C-463C-9BF8-C1E65C7DE49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E5C7D-04FF-410B-84F9-45CD12F791E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -162,26 +162,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -501,7 +500,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,13 +530,13 @@
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -558,14 +557,14 @@
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="5"/>
-      <c r="K2" s="9"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -586,20 +585,20 @@
       <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="5"/>
-      <c r="K3" s="9"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
@@ -618,11 +617,11 @@
       <c r="H4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>632723300011</v>
       </c>
       <c r="J4" s="5"/>
-      <c r="K4" s="9"/>
+      <c r="K4" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update parts list with bom and other pricing
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E5C7D-04FF-410B-84F9-45CD12F791E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0A2ED0-2886-4E2C-B57C-65CD0F18C313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Price</t>
   </si>
@@ -88,6 +88,87 @@
   </si>
   <si>
     <t>D73-N52</t>
+  </si>
+  <si>
+    <t>Preliminary BOM</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>2906-4-15-20-75-14-11-0</t>
+  </si>
+  <si>
+    <t>54-2906-4-15-20-75-14-11-0-ND</t>
+  </si>
+  <si>
+    <t>Digikey SKU</t>
+  </si>
+  <si>
+    <t>Manufacturer SKU</t>
+  </si>
+  <si>
+    <t>Mill-Max</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>GuHua</t>
+  </si>
+  <si>
+    <t>Aliexpress Heat Set Inserts</t>
+  </si>
+  <si>
+    <t>Female Half</t>
+  </si>
+  <si>
+    <t>Male Half</t>
+  </si>
+  <si>
+    <t>PCBWay</t>
+  </si>
+  <si>
+    <t>Printed Parts</t>
+  </si>
+  <si>
+    <t>Filament</t>
+  </si>
+  <si>
+    <t>Gen. ASA</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Estimated Amount (g)</t>
+  </si>
+  <si>
+    <t>K&amp;J Magnetics</t>
+  </si>
+  <si>
+    <t>Equipment Tracking</t>
+  </si>
+  <si>
+    <t>Soldering Plate</t>
+  </si>
+  <si>
+    <t>Solder Paste</t>
+  </si>
+  <si>
+    <t>Flux Paste</t>
+  </si>
+  <si>
+    <t>Prelim. BOM Total</t>
   </si>
 </sst>
 </file>
@@ -137,12 +218,40 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -151,7 +260,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -181,6 +290,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -497,17 +623,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0D2EA4-1276-4D7D-AD5E-6C96E3844A7C}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="5"/>
     <col min="5" max="5" width="9.140625" style="3"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
@@ -623,9 +749,277 @@
       <c r="J4" s="5"/>
       <c r="K4" s="8"/>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="H7" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="19">
+        <f>SUM(F:F)</f>
+        <v>36.926000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="F9" s="18">
+        <f>E9*D9</f>
+        <v>8.9600000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="F10" s="18">
+        <f>E10*D10</f>
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F11" s="18">
+        <f>E11*D11</f>
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3">
+        <f>1.35</f>
+        <v>1.35</v>
+      </c>
+      <c r="F12" s="18">
+        <f>E12*D12</f>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10</v>
+      </c>
+      <c r="F13" s="18">
+        <f>E13*D13</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f>(25/2000)*C16</f>
+        <v>0.125</v>
+      </c>
+      <c r="F16" s="18">
+        <f>D16*E16</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <f>(25/2000)*C17</f>
+        <v>0.125</v>
+      </c>
+      <c r="F17" s="18">
+        <f>D17*E17</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="3">
+        <v>24.93</v>
+      </c>
+      <c r="C22" s="21">
+        <f>SUM(B22:B32)</f>
+        <v>36.130000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{5C8C6655-FD90-46E5-A3A0-60445F66EAFE}"/>

</xml_diff>

<commit_message>
added quick final files before home
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0A2ED0-2886-4E2C-B57C-65CD0F18C313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676874F6-3337-4E96-883C-857D0CCC4BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Price</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Prelim. BOM Total</t>
+  </si>
+  <si>
+    <t>D83-N52</t>
   </si>
 </sst>
 </file>
@@ -287,16 +290,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,6 +304,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -626,7 +629,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,11 +659,11 @@
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
@@ -725,17 +728,17 @@
         <v>16</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5">
         <v>4</v>
       </c>
       <c r="E4" s="3">
-        <f>D4*1.35</f>
-        <v>5.4</v>
+        <f>1.71</f>
+        <v>1.71</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>5</v>
@@ -750,40 +753,40 @@
       <c r="K4" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="H7" s="15" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="H7" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="17">
         <f>SUM(F:F)</f>
-        <v>36.926000000000002</v>
+        <v>38.366</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -802,7 +805,7 @@
       <c r="E9" s="3">
         <v>0.64</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <f>E9*D9</f>
         <v>8.9600000000000009</v>
       </c>
@@ -814,7 +817,7 @@
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="5">
@@ -823,7 +826,7 @@
       <c r="E10" s="3">
         <v>0.97</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <f>E10*D10</f>
         <v>1.94</v>
       </c>
@@ -844,7 +847,7 @@
       <c r="E11" s="3">
         <v>4.7E-2</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f>E11*D11</f>
         <v>0.376</v>
       </c>
@@ -863,12 +866,12 @@
         <v>4</v>
       </c>
       <c r="E12" s="3">
-        <f>1.35</f>
-        <v>1.35</v>
-      </c>
-      <c r="F12" s="18">
+        <f>E4</f>
+        <v>1.71</v>
+      </c>
+      <c r="F12" s="16">
         <f>E12*D12</f>
-        <v>5.4</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -887,38 +890,38 @@
       <c r="E13" s="3">
         <v>10</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="16">
         <f>E13*D13</f>
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -939,7 +942,7 @@
         <f>(25/2000)*C16</f>
         <v>0.125</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="16">
         <f>D16*E16</f>
         <v>0.125</v>
       </c>
@@ -961,25 +964,25 @@
         <f>(25/2000)*C17</f>
         <v>0.125</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="16">
         <f>D17*E17</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="21"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -990,7 +993,7 @@
       <c r="B22" s="3">
         <v>24.93</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="19">
         <f>SUM(B22:B32)</f>
         <v>36.130000000000003</v>
       </c>

</xml_diff>

<commit_message>
corrected magnet type in parts list
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676874F6-3337-4E96-883C-857D0CCC4BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8839EFC-9928-428C-8163-E8B24927CBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Price</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>K&amp;J Magnets</t>
-  </si>
-  <si>
-    <t>D73-N52</t>
   </si>
   <si>
     <t>Preliminary BOM</t>
@@ -629,7 +626,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,10 +725,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="5">
         <v>4</v>
@@ -754,7 +751,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -762,18 +759,18 @@
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="H7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>4</v>
@@ -782,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="17">
         <f>SUM(F:F)</f>
@@ -791,13 +788,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="5">
         <v>14</v>
@@ -812,7 +809,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -833,13 +830,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5">
         <v>8</v>
@@ -854,13 +851,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
@@ -876,13 +873,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="5">
         <v>2</v>
@@ -897,7 +894,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -907,13 +904,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>4</v>
@@ -922,15 +919,15 @@
         <v>0</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -949,10 +946,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -971,7 +968,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="21"/>
     </row>
@@ -983,12 +980,12 @@
         <v>0</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3">
         <v>24.93</v>
@@ -1000,7 +997,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="3">
         <v>7.1</v>
@@ -1008,7 +1005,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="3">
         <v>4.0999999999999996</v>

</xml_diff>

<commit_message>
rev2 of boards plus compliant bom
The female connector has been updated with larger pads for better slop
compensation.

A BOM matching the PCBWay format has been implemented for each part to
aid in manufacturing/assembly.
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8839EFC-9928-428C-8163-E8B24927CBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738C11E6-D3C2-46B1-87C7-2941523B47EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
+    <workbookView xWindow="11700" yWindow="0" windowWidth="17100" windowHeight="15600" xr2:uid="{0FA53072-6918-4FD0-8585-E345289BF28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>